<commit_message>
changes to deposito a plazo
</commit_message>
<xml_diff>
--- a/0c963a043f92e3c567b6afb48d406df5a2f38f5c/depositos_a_plazo.xlsx
+++ b/0c963a043f92e3c567b6afb48d406df5a2f38f5c/depositos_a_plazo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Alvacast\Curso\0c963a043f92e3c567b6afb48d406df5a2f38f5c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB015F09-C44E-49F3-B317-96A7A6858C8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C417B11-9E66-49C8-9242-A7CAC9811AD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15972" xr2:uid="{9D5C85E2-BCAA-4DAB-88D3-E7938B7E5077}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Vigentes</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>monto_vencimiento</t>
+  </si>
+  <si>
+    <t>orden</t>
   </si>
 </sst>
 </file>
@@ -440,20 +443,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED3109C-3290-4CAB-8522-1F8BA477610B}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="1" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -461,121 +464,148 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
         <v>251472</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>252200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
         <v>1005795</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>1008799</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
         <v>4035947</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>4048754</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4">
         <v>514349</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>517229</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
         <v>1065968</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>1068953</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4">
         <v>534917</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>536415</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4">
         <v>548554</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>550192</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4">
         <v>1651446</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>1706935</v>
       </c>
     </row>

</xml_diff>